<commit_message>
possbility to save prediction of each model inside a csv file, to backtesdt
</commit_message>
<xml_diff>
--- a/saved_model/specs/15_min.xlsx
+++ b/saved_model/specs/15_min.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>delay</t>
   </si>
@@ -52,19 +52,16 @@
     <t>20200101</t>
   </si>
   <si>
-    <t>20200731</t>
-  </si>
-  <si>
-    <t>33%</t>
-  </si>
-  <si>
-    <t>5%</t>
-  </si>
-  <si>
-    <t>34%</t>
-  </si>
-  <si>
-    <t>18%</t>
+    <t>20210130</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>47%</t>
+  </si>
+  <si>
+    <t>40%</t>
   </si>
 </sst>
 </file>
@@ -396,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -442,7 +439,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.5891647855530474</v>
+        <v>0.5532819558862609</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -469,7 +466,7 @@
         <v>25</v>
       </c>
       <c r="K2">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -477,7 +474,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.665</v>
+        <v>0.5500495540138751</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -498,83 +495,13 @@
         <v>0.05</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J3">
         <v>25</v>
       </c>
       <c r="K3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0.5496402877697841</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4">
-        <v>30</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4">
-        <v>0.8</v>
-      </c>
-      <c r="H4">
-        <v>0.05</v>
-      </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4">
-        <v>25</v>
-      </c>
-      <c r="K4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>0.601078167115903</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>30</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5">
-        <v>0.8</v>
-      </c>
-      <c r="H5">
-        <v>0.05</v>
-      </c>
-      <c r="I5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5">
-        <v>25</v>
-      </c>
-      <c r="K5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>